<commit_message>
Procesamiento con la BD.
Se modifica la vista principal para agregar menú de importación.
Se termina procesamiento de archivo excel para 1 curso.
Se crea excel con datos reales para prueba de 1 curso.
</commit_message>
<xml_diff>
--- a/cpruebas.pruebas/src/multi_1A.xlsx
+++ b/cpruebas.pruebas/src/multi_1A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cpruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>idColegio</t>
   </si>
@@ -41,52 +41,200 @@
     <t>respuestas</t>
   </si>
   <si>
-    <t>24330328-1</t>
-  </si>
-  <si>
-    <t>24407661-0</t>
-  </si>
-  <si>
-    <t>24433888-7</t>
-  </si>
-  <si>
-    <t>24528698-8</t>
-  </si>
-  <si>
-    <t>24558220-K</t>
-  </si>
-  <si>
-    <t>24588886-4</t>
-  </si>
-  <si>
-    <t>24666681-4</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>CCC</t>
-  </si>
-  <si>
-    <t>DDD</t>
-  </si>
-  <si>
-    <t>EEE</t>
-  </si>
-  <si>
-    <t>FFF</t>
-  </si>
-  <si>
-    <t>GGG</t>
+    <t>21709062-8</t>
+  </si>
+  <si>
+    <t>21616257-9</t>
+  </si>
+  <si>
+    <t>21742548-4</t>
+  </si>
+  <si>
+    <t>21643856-6</t>
+  </si>
+  <si>
+    <t>21697382-8</t>
+  </si>
+  <si>
+    <t>21797036-9</t>
+  </si>
+  <si>
+    <t>21862419-7</t>
+  </si>
+  <si>
+    <t>BDACBCABCDCCDABBCABACDDDB</t>
+  </si>
+  <si>
+    <t>21665540-0</t>
+  </si>
+  <si>
+    <t>BDBOADBCADCADADACDBCADBCA</t>
+  </si>
+  <si>
+    <t>21864781-2</t>
+  </si>
+  <si>
+    <t>OACBDDACCDCBOAABCCBAACCBB</t>
+  </si>
+  <si>
+    <t>21598050-2</t>
+  </si>
+  <si>
+    <t>CBBCBCABCDABDABDCAAABDBBB</t>
+  </si>
+  <si>
+    <t>21758392-6</t>
+  </si>
+  <si>
+    <t>BCBCDADBCADBCBDBDBDACBDBD</t>
+  </si>
+  <si>
+    <t>21671455-5</t>
+  </si>
+  <si>
+    <t>BCBBDADAADBCCABDCCDAABBDB</t>
+  </si>
+  <si>
+    <t>21753188-8</t>
+  </si>
+  <si>
+    <t>BADBCDCDCDADBCACADAACCBBB</t>
+  </si>
+  <si>
+    <t>21832400-2</t>
+  </si>
+  <si>
+    <t>BADBCDCDCAADBADBCCAAABBDB</t>
+  </si>
+  <si>
+    <t>21828371-3</t>
+  </si>
+  <si>
+    <t>BDCCDACDBADDCCACCABDACBCA</t>
+  </si>
+  <si>
+    <t>21681052-k</t>
+  </si>
+  <si>
+    <t>CABAABDACBDACBADACBDBDDAB</t>
+  </si>
+  <si>
+    <t>21643418-8</t>
+  </si>
+  <si>
+    <t>BBBBDDDACDAAABBABCDAAABBB</t>
+  </si>
+  <si>
+    <t>21652955-3</t>
+  </si>
+  <si>
+    <t>DCBBAAACCDCDDBBACBBAAABDB</t>
+  </si>
+  <si>
+    <t>21658868-1</t>
+  </si>
+  <si>
+    <t>BDDBABCACBCBDADBDCAADCADB</t>
+  </si>
+  <si>
+    <t>21631042-K</t>
+  </si>
+  <si>
+    <t>BCDBDBCDCDCCAAAACCAACADAB</t>
+  </si>
+  <si>
+    <t>21646689-1</t>
+  </si>
+  <si>
+    <t>BCDCAACBDDBCADACCADBBBCDB</t>
+  </si>
+  <si>
+    <t>21822820-8</t>
+  </si>
+  <si>
+    <t>BCABDBDACBCABADCACBDACBDC</t>
+  </si>
+  <si>
+    <t>21821201-8</t>
+  </si>
+  <si>
+    <t>BCDBDBCACDDDBBDCBACACCCDB</t>
+  </si>
+  <si>
+    <t>21624805-8</t>
+  </si>
+  <si>
+    <t>CDBDDDDCCDBDCAABCCBACCBDB</t>
+  </si>
+  <si>
+    <t>BCADCBCBDDABDDADCADCCDBDB</t>
+  </si>
+  <si>
+    <t>BBBBDCBDACADBAADCCABCCCAB</t>
+  </si>
+  <si>
+    <t>21620974-5</t>
+  </si>
+  <si>
+    <t>BDBBDBCDCDBDADDBACBACCBDB</t>
+  </si>
+  <si>
+    <t>21605465-2</t>
+  </si>
+  <si>
+    <t>BOACBOCCBDBDABDBDAACCBBDB</t>
+  </si>
+  <si>
+    <t>21491569-3</t>
+  </si>
+  <si>
+    <t>ACAACDCACDBDCACBDBMBCACAD</t>
+  </si>
+  <si>
+    <t>BBBODOOCCDAAABBCCABACCBDB</t>
+  </si>
+  <si>
+    <t>21822377-k</t>
+  </si>
+  <si>
+    <t>BABCABDACBADABABACADACDBA</t>
+  </si>
+  <si>
+    <t>BCDBDACDADBDCBCADBCADCDCA</t>
+  </si>
+  <si>
+    <t>21831683-2</t>
+  </si>
+  <si>
+    <t>BCBCDBCCDABDADBACCBDBABBB</t>
+  </si>
+  <si>
+    <t>BDACBCABCDCBDABBDCABCDCAB</t>
+  </si>
+  <si>
+    <t>21833092-4</t>
+  </si>
+  <si>
+    <t>BBCDBBDBBDCBAABDACBAADDCB</t>
+  </si>
+  <si>
+    <t>21714954-1</t>
+  </si>
+  <si>
+    <t>ACBDACBDACABBCADBCADACBDA</t>
+  </si>
+  <si>
+    <t>CBABDBCBCBBCDOBCBDBACBCCC</t>
+  </si>
+  <si>
+    <t>CBABDBCBCBBCDOBCBDBACBCBB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,12 +244,60 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,11 +312,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,15 +601,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="34.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -431,121 +632,546 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B2">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B3">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B4">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B5">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B6">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B7">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="B8">
-        <v>982</v>
+        <v>10040</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10000</v>
+      </c>
+      <c r="B9">
+        <v>10040</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10000</v>
+      </c>
+      <c r="B10">
+        <v>10040</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10000</v>
+      </c>
+      <c r="B11">
+        <v>10040</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10000</v>
+      </c>
+      <c r="B12">
+        <v>10040</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10000</v>
+      </c>
+      <c r="B13">
+        <v>10040</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10000</v>
+      </c>
+      <c r="B14">
+        <v>10040</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10000</v>
+      </c>
+      <c r="B15">
+        <v>10040</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10000</v>
+      </c>
+      <c r="B16">
+        <v>10040</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10000</v>
+      </c>
+      <c r="B17">
+        <v>10040</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10000</v>
+      </c>
+      <c r="B18">
+        <v>10040</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>10040</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10000</v>
+      </c>
+      <c r="B20">
+        <v>10040</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10000</v>
+      </c>
+      <c r="B21">
+        <v>10040</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10000</v>
+      </c>
+      <c r="B22">
+        <v>10040</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10000</v>
+      </c>
+      <c r="B23">
+        <v>10040</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10000</v>
+      </c>
+      <c r="B24">
+        <v>10040</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10000</v>
+      </c>
+      <c r="B25">
+        <v>10040</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10000</v>
+      </c>
+      <c r="B26">
+        <v>10040</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10000</v>
+      </c>
+      <c r="B27">
+        <v>10040</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10000</v>
+      </c>
+      <c r="B28">
+        <v>10040</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10000</v>
+      </c>
+      <c r="B29">
+        <v>10040</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10000</v>
+      </c>
+      <c r="B30">
+        <v>10040</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10000</v>
+      </c>
+      <c r="B31">
+        <v>10040</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10000</v>
+      </c>
+      <c r="B32">
+        <v>10040</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10000</v>
+      </c>
+      <c r="B33">
+        <v>10040</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>